<commit_message>
dossier data + readme
</commit_message>
<xml_diff>
--- a/01_doc/Comparaison des temps d'exécutions au sein de la boucle de auto mode.xlsx
+++ b/01_doc/Comparaison des temps d'exécutions au sein de la boucle de auto mode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Stage_1DOF_DroneBench\01_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660E90C0-C9B3-47FB-8999-B107964CFF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74206178-5B56-479F-AFF5-8E3226E56D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{42F1FBAE-4704-47C6-9EC6-A37202DDD779}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42F1FBAE-4704-47C6-9EC6-A37202DDD779}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -950,7 +950,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2772,10 +2771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949861EA-E65B-4FA2-BB9E-0FB2D8D9864F}">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2905,6 +2904,12 @@
       <c r="C18">
         <f>C16/C13</f>
         <v>1210.612266262671</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f>7250/10000</f>
+        <v>0.72499999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2979,7 +2984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7ADD59F-C9B3-4ABB-AC02-AD4B4B51F911}">
   <dimension ref="A2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>